<commit_message>
Fix device connection issues
</commit_message>
<xml_diff>
--- a/devnet_sbx_testbed.xlsx
+++ b/devnet_sbx_testbed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudia/Dropbox (Indigo Wire Networks)/scripts/python/2020/pyats_intro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkruliv/Documents/Work/ONC/pyATS/pyats_intro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA673185-3A3C-0441-8E37-F28732172CB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F031A263-B188-4A4D-96FD-6A6155DF2123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9440" yWindow="9280" windowWidth="28040" windowHeight="17440" xr2:uid="{B1CD2092-96F8-D541-AB83-A29EF0B7CE1F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{B1CD2092-96F8-D541-AB83-A29EF0B7CE1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -56,18 +48,12 @@
     <t>port</t>
   </si>
   <si>
-    <t>sbx-n9kv-ao</t>
-  </si>
-  <si>
     <t>csr1000v-1</t>
   </si>
   <si>
     <t>sbx-nxos-mgmt.cisco.com</t>
   </si>
   <si>
-    <t>ios-xe-mgmt-latest.cisco.com</t>
-  </si>
-  <si>
     <t>ssh</t>
   </si>
   <si>
@@ -90,6 +76,12 @@
   </si>
   <si>
     <t>developer</t>
+  </si>
+  <si>
+    <t>sbx-ao</t>
+  </si>
+  <si>
+    <t>ios-xe-mgmt.cisco.com</t>
   </si>
 </sst>
 </file>
@@ -444,7 +436,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,7 +459,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -481,54 +473,54 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
       <c r="G2">
         <v>8181</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>8181</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>